<commit_message>
Use "framework" more consistently.
</commit_message>
<xml_diff>
--- a/Framework.xlsx
+++ b/Framework.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nistgov.sharepoint.com/sites/staff/Performance assurance/Shared Documents/Knowledge Base + IRAF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/libes/Desktop/iraf feedback/mfgkb/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Framework" sheetId="14" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171026" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -613,16 +613,37 @@
 Transmission Control, Impacts, and Formats</t>
   </si>
   <si>
+    <t>Integrity: Ensure information is communicated with agreed acceptable loss of information.</t>
+  </si>
+  <si>
     <t>Protect information from corruption.</t>
   </si>
   <si>
+    <t>Define acceptable loss of information.</t>
+  </si>
+  <si>
+    <t>Ensure required signal strength.</t>
+  </si>
+  <si>
     <t>Control interference within agreed limits to transmission (e.g., crosstalk).</t>
   </si>
   <si>
-    <t>Ensure required signal strength.</t>
-  </si>
-  <si>
-    <t>Define acceptable loss of information.</t>
+    <t>Ensure consistent syntax (formats, protocols) appropriate for all relevant systems.</t>
+  </si>
+  <si>
+    <t>Integration: Ensure interoperability of information.</t>
+  </si>
+  <si>
+    <t>Ensure and document syntactic interoperability. Document deviations.</t>
+  </si>
+  <si>
+    <t>Ensure and document symantic interoperability. Document deviations.</t>
+  </si>
+  <si>
+    <t>Use widely-accepted standards to support diverse sources of information.</t>
+  </si>
+  <si>
+    <t>Multiple conflicting standards or lack of agreement on which standards to use. Some standards are proprietary.</t>
   </si>
   <si>
     <t>Information Availability and Timeliness: Ensure information is available and ready for transmission when requested. Ensure arrival within time needed.</t>
@@ -637,12 +658,24 @@
     <t>Provide an extensible transmission infrastructure to accommodate improvement and expansion.</t>
   </si>
   <si>
+    <t>Provenance and Certification: Provide traceability and roots of trust.</t>
+  </si>
+  <si>
+    <t>Document traceability and certification requirements and mechanisms.</t>
+  </si>
+  <si>
+    <t>Enact traceability and certification functionality.</t>
+  </si>
+  <si>
     <t>Cybersecurity: Ensure security of transmission systems consistent with organization's security strategies, policies, and procedures.</t>
   </si>
   <si>
     <t>Document security policies and procedures.</t>
   </si>
   <si>
+    <t>Establish procedures to manage security consistent with requirements and priorities</t>
+  </si>
+  <si>
     <t>Install and regularly test security procedures.</t>
   </si>
   <si>
@@ -652,16 +685,16 @@
     <t>Adapt transmission systems to adhere with changing strategies, policies, and procedures.</t>
   </si>
   <si>
+    <t>Establish procedures to manage infrastructure consistent with requirements and priorities</t>
+  </si>
+  <si>
     <t>Manufacturing Operations Interactions: Ensure information transmission impacts on operations of organization are understood.</t>
   </si>
   <si>
     <t>Document transmission impacts.</t>
   </si>
   <si>
-    <t>Use widely-accepted standards to support diverse sources of information.</t>
-  </si>
-  <si>
-    <t>Multiple conflicting standards or lack of agreement on which standards to use. Some standards are proprietary.</t>
+    <t>Establish limits to interactions and procedures to address and manage any potential interactions beyond agreed-upon limits.</t>
   </si>
   <si>
     <t>ANALYZE
@@ -1255,39 +1288,6 @@
   </si>
   <si>
     <t>All data cells (B- and 2- and higher) use ChecklistData format.</t>
-  </si>
-  <si>
-    <t>Provenance and Certification: Provide traceability and roots of trust.</t>
-  </si>
-  <si>
-    <t>Document traceability and certification requirements and mechanisms.</t>
-  </si>
-  <si>
-    <t>Enact traceability and certification functionality.</t>
-  </si>
-  <si>
-    <t>Integration: Ensure interoperability of information.</t>
-  </si>
-  <si>
-    <t>Integrity: Ensure information is communicated with agreed acceptable loss of information.</t>
-  </si>
-  <si>
-    <t>Ensure consistent syntax (formats, protocols) appropriate for all relevant systems.</t>
-  </si>
-  <si>
-    <t>Ensure and document syntactic interoperability. Document deviations.</t>
-  </si>
-  <si>
-    <t>Ensure and document symantic interoperability. Document deviations.</t>
-  </si>
-  <si>
-    <t>Establish procedures to manage infrastructure consistent with requirements and priorities</t>
-  </si>
-  <si>
-    <t>Establish procedures to manage security consistent with requirements and priorities</t>
-  </si>
-  <si>
-    <t>Establish limits to interactions and procedures to address and manage any potential interactions beyond agreed-upon limits.</t>
   </si>
 </sst>
 </file>
@@ -1577,6 +1577,15 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="14" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1586,35 +1595,26 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="15" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="ChecklistData" xfId="14"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Function" xfId="15"/>
     <cellStyle name="Headers" xfId="16"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1922,7 +1922,7 @@
   <dimension ref="A1:BB205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B179" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B183" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C197" sqref="C197"/>
@@ -4894,7 +4894,7 @@
       <c r="BB65" s="17"/>
     </row>
     <row r="66" spans="1:54" ht="32" x14ac:dyDescent="0.2">
-      <c r="A66" s="28" t="s">
+      <c r="A66" s="25" t="s">
         <v>147</v>
       </c>
       <c r="B66" s="24" t="s">
@@ -4913,7 +4913,7 @@
       <c r="G66" s="14"/>
     </row>
     <row r="67" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="29"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="24"/>
       <c r="C67" s="10" t="s">
         <v>152</v>
@@ -4928,7 +4928,7 @@
       <c r="G67" s="14"/>
     </row>
     <row r="68" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="29"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="24"/>
       <c r="C68" s="10" t="s">
         <v>155</v>
@@ -4943,7 +4943,7 @@
       <c r="G68" s="14"/>
     </row>
     <row r="69" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="29"/>
+      <c r="A69" s="26"/>
       <c r="B69" s="24"/>
       <c r="C69" s="10" t="s">
         <v>157</v>
@@ -4956,7 +4956,7 @@
       <c r="G69" s="14"/>
     </row>
     <row r="70" spans="1:54" ht="32" x14ac:dyDescent="0.2">
-      <c r="A70" s="29"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="24"/>
       <c r="C70" s="10" t="s">
         <v>159</v>
@@ -4971,7 +4971,7 @@
       <c r="G70" s="14"/>
     </row>
     <row r="71" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="29"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="24"/>
       <c r="C71" s="10" t="s">
         <v>162</v>
@@ -4982,7 +4982,7 @@
       <c r="G71" s="14"/>
     </row>
     <row r="72" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="29"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="24" t="s">
         <v>163</v>
       </c>
@@ -4995,7 +4995,7 @@
       <c r="G72" s="14"/>
     </row>
     <row r="73" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="29"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="24"/>
       <c r="C73" s="10" t="s">
         <v>165</v>
@@ -5006,7 +5006,7 @@
       <c r="G73" s="14"/>
     </row>
     <row r="74" spans="1:54" ht="32" x14ac:dyDescent="0.2">
-      <c r="A74" s="29"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="24" t="s">
         <v>166</v>
       </c>
@@ -5021,7 +5021,7 @@
       <c r="G74" s="14"/>
     </row>
     <row r="75" spans="1:54" ht="32" x14ac:dyDescent="0.2">
-      <c r="A75" s="29"/>
+      <c r="A75" s="26"/>
       <c r="B75" s="24"/>
       <c r="C75" s="10" t="s">
         <v>169</v>
@@ -5034,7 +5034,7 @@
       <c r="G75" s="14"/>
     </row>
     <row r="76" spans="1:54" ht="32" x14ac:dyDescent="0.2">
-      <c r="A76" s="29"/>
+      <c r="A76" s="26"/>
       <c r="B76" s="24"/>
       <c r="C76" s="10" t="s">
         <v>171</v>
@@ -5047,7 +5047,7 @@
       <c r="G76" s="14"/>
     </row>
     <row r="77" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="29"/>
+      <c r="A77" s="26"/>
       <c r="B77" s="24"/>
       <c r="C77" s="10" t="s">
         <v>173</v>
@@ -5060,7 +5060,7 @@
       <c r="G77" s="14"/>
     </row>
     <row r="78" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="29"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="24" t="s">
         <v>175</v>
       </c>
@@ -5075,7 +5075,7 @@
       <c r="G78" s="14"/>
     </row>
     <row r="79" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="29"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="24"/>
       <c r="C79" s="10" t="s">
         <v>178</v>
@@ -5088,7 +5088,7 @@
       <c r="G79" s="14"/>
     </row>
     <row r="80" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="29"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="24"/>
       <c r="C80" s="10" t="s">
         <v>180</v>
@@ -5099,7 +5099,7 @@
       <c r="G80" s="14"/>
     </row>
     <row r="81" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" s="29"/>
+      <c r="A81" s="26"/>
       <c r="B81" s="24"/>
       <c r="C81" s="10" t="s">
         <v>181</v>
@@ -5110,7 +5110,7 @@
       <c r="G81" s="14"/>
     </row>
     <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="30"/>
+      <c r="A82" s="27"/>
       <c r="B82" s="24"/>
       <c r="C82" s="10" t="s">
         <v>182</v>
@@ -5123,14 +5123,14 @@
       <c r="G82" s="14"/>
     </row>
     <row r="83" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="28" t="s">
+      <c r="A83" s="25" t="s">
         <v>184</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>402</v>
+        <v>185</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D83" s="10"/>
       <c r="E83" s="10"/>
@@ -5138,10 +5138,10 @@
       <c r="G83" s="14"/>
     </row>
     <row r="84" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="29"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="23"/>
       <c r="C84" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
@@ -5149,10 +5149,10 @@
       <c r="G84" s="14"/>
     </row>
     <row r="85" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A85" s="29"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="23"/>
       <c r="C85" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D85" s="10"/>
       <c r="E85" s="10"/>
@@ -5160,10 +5160,10 @@
       <c r="G85" s="14"/>
     </row>
     <row r="86" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="29"/>
+      <c r="A86" s="26"/>
       <c r="B86" s="23"/>
       <c r="C86" s="10" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D86" s="10"/>
       <c r="E86" s="10"/>
@@ -5171,10 +5171,10 @@
       <c r="G86" s="14"/>
     </row>
     <row r="87" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="29"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="22"/>
       <c r="C87" s="10" t="s">
-        <v>403</v>
+        <v>190</v>
       </c>
       <c r="D87" s="10"/>
       <c r="E87" s="10"/>
@@ -5182,12 +5182,12 @@
       <c r="G87" s="14"/>
     </row>
     <row r="88" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="29"/>
+      <c r="A88" s="26"/>
       <c r="B88" s="21" t="s">
-        <v>401</v>
+        <v>191</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>404</v>
+        <v>192</v>
       </c>
       <c r="D88" s="10"/>
       <c r="E88" s="10"/>
@@ -5195,10 +5195,10 @@
       <c r="G88" s="14"/>
     </row>
     <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="29"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="23"/>
       <c r="C89" s="10" t="s">
-        <v>405</v>
+        <v>193</v>
       </c>
       <c r="D89" s="10"/>
       <c r="E89" s="10"/>
@@ -5206,25 +5206,25 @@
       <c r="G89" s="14"/>
     </row>
     <row r="90" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="29"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="23"/>
       <c r="C90" s="10" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E90" s="10"/>
       <c r="F90" s="14"/>
       <c r="G90" s="14"/>
     </row>
     <row r="91" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A91" s="29"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="24" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D91" s="10"/>
       <c r="E91" s="10"/>
@@ -5232,10 +5232,10 @@
       <c r="G91" s="14"/>
     </row>
     <row r="92" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="29"/>
+      <c r="A92" s="26"/>
       <c r="B92" s="24"/>
       <c r="C92" s="10" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="D92" s="10"/>
       <c r="E92" s="10"/>
@@ -5243,10 +5243,10 @@
       <c r="G92" s="14"/>
     </row>
     <row r="93" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A93" s="29"/>
+      <c r="A93" s="26"/>
       <c r="B93" s="24"/>
       <c r="C93" s="10" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D93" s="10"/>
       <c r="E93" s="10"/>
@@ -5254,12 +5254,12 @@
       <c r="G93" s="14"/>
     </row>
     <row r="94" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="29"/>
+      <c r="A94" s="26"/>
       <c r="B94" s="24" t="s">
-        <v>398</v>
+        <v>200</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>399</v>
+        <v>201</v>
       </c>
       <c r="D94" s="10"/>
       <c r="E94" s="10"/>
@@ -5267,10 +5267,10 @@
       <c r="G94" s="14"/>
     </row>
     <row r="95" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95" s="29"/>
+      <c r="A95" s="26"/>
       <c r="B95" s="24"/>
       <c r="C95" s="10" t="s">
-        <v>400</v>
+        <v>202</v>
       </c>
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
@@ -5278,12 +5278,12 @@
       <c r="G95" s="14"/>
     </row>
     <row r="96" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="29"/>
+      <c r="A96" s="26"/>
       <c r="B96" s="21" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D96" s="10"/>
       <c r="E96" s="10"/>
@@ -5291,10 +5291,10 @@
       <c r="G96" s="14"/>
     </row>
     <row r="97" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A97" s="29"/>
+      <c r="A97" s="26"/>
       <c r="B97" s="23"/>
       <c r="C97" s="10" t="s">
-        <v>407</v>
+        <v>205</v>
       </c>
       <c r="D97" s="10"/>
       <c r="E97" s="10"/>
@@ -5302,10 +5302,10 @@
       <c r="G97" s="14"/>
     </row>
     <row r="98" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="29"/>
+      <c r="A98" s="26"/>
       <c r="B98" s="22"/>
       <c r="C98" s="10" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="D98" s="10"/>
       <c r="E98" s="10"/>
@@ -5313,12 +5313,12 @@
       <c r="G98" s="14"/>
     </row>
     <row r="99" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A99" s="29"/>
+      <c r="A99" s="26"/>
       <c r="B99" s="21" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="D99" s="10"/>
       <c r="E99" s="10"/>
@@ -5326,10 +5326,10 @@
       <c r="G99" s="14"/>
     </row>
     <row r="100" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A100" s="29"/>
+      <c r="A100" s="26"/>
       <c r="B100" s="22"/>
       <c r="C100" s="10" t="s">
-        <v>406</v>
+        <v>209</v>
       </c>
       <c r="D100" s="10"/>
       <c r="E100" s="10"/>
@@ -5337,12 +5337,12 @@
       <c r="G100" s="14"/>
     </row>
     <row r="101" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="29"/>
+      <c r="A101" s="26"/>
       <c r="B101" s="21" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="D101" s="10"/>
       <c r="E101" s="10"/>
@@ -5350,10 +5350,10 @@
       <c r="G101" s="14"/>
     </row>
     <row r="102" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A102" s="29"/>
+      <c r="A102" s="26"/>
       <c r="B102" s="22"/>
       <c r="C102" s="10" t="s">
-        <v>408</v>
+        <v>212</v>
       </c>
       <c r="D102" s="10"/>
       <c r="E102" s="10"/>
@@ -5361,312 +5361,312 @@
       <c r="G102" s="14"/>
     </row>
     <row r="103" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="25" t="s">
-        <v>202</v>
+      <c r="A103" s="28" t="s">
+        <v>213</v>
       </c>
       <c r="B103" s="24" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="E103" s="10" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="F103" s="10" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="G103" s="14"/>
     </row>
     <row r="104" spans="1:7" ht="80" x14ac:dyDescent="0.2">
-      <c r="A104" s="26"/>
+      <c r="A104" s="29"/>
       <c r="B104" s="24"/>
       <c r="C104" s="10" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="E104" s="10" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="F104" s="10" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="G104" s="14"/>
     </row>
     <row r="105" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="26"/>
+      <c r="A105" s="29"/>
       <c r="B105" s="24"/>
       <c r="C105" s="10" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="E105" s="10"/>
       <c r="F105" s="10" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="G105" s="14"/>
     </row>
     <row r="106" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="26"/>
+      <c r="A106" s="29"/>
       <c r="B106" s="24"/>
       <c r="C106" s="10" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="E106" s="10" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="F106" s="10"/>
       <c r="G106" s="14"/>
     </row>
     <row r="107" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A107" s="26"/>
+      <c r="A107" s="29"/>
       <c r="B107" s="24"/>
       <c r="C107" s="10" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="E107" s="10"/>
       <c r="F107" s="10" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="G107" s="14"/>
     </row>
     <row r="108" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A108" s="26"/>
+      <c r="A108" s="29"/>
       <c r="B108" s="24"/>
       <c r="C108" s="10" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="E108" s="10" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="F108" s="10" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="G108" s="14"/>
     </row>
     <row r="109" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="26"/>
+      <c r="A109" s="29"/>
       <c r="B109" s="24" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C109" s="24" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="E109" s="10" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="F109" s="10"/>
       <c r="G109" s="14"/>
     </row>
     <row r="110" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A110" s="26"/>
+      <c r="A110" s="29"/>
       <c r="B110" s="24"/>
       <c r="C110" s="24"/>
       <c r="D110" s="10" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="E110" s="10" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="F110" s="10"/>
       <c r="G110" s="14"/>
     </row>
     <row r="111" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A111" s="26"/>
+      <c r="A111" s="29"/>
       <c r="B111" s="24"/>
       <c r="C111" s="24" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="E111" s="10" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F111" s="10" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="G111" s="14"/>
     </row>
     <row r="112" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A112" s="26"/>
+      <c r="A112" s="29"/>
       <c r="B112" s="24"/>
       <c r="C112" s="24"/>
       <c r="D112" s="10" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="E112" s="10"/>
       <c r="F112" s="10"/>
       <c r="G112" s="14"/>
     </row>
     <row r="113" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A113" s="26"/>
+      <c r="A113" s="29"/>
       <c r="B113" s="24"/>
       <c r="C113" s="10" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="D113" s="10" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="E113" s="10"/>
       <c r="F113" s="10"/>
       <c r="G113" s="10" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="26"/>
+      <c r="A114" s="29"/>
       <c r="B114" s="24"/>
       <c r="C114" s="10" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="D114" s="10" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="E114" s="10"/>
       <c r="F114" s="10"/>
       <c r="G114" s="14"/>
     </row>
     <row r="115" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A115" s="26"/>
+      <c r="A115" s="29"/>
       <c r="B115" s="24"/>
       <c r="C115" s="10" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="D115" s="10" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="E115" s="10" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="F115" s="10"/>
       <c r="G115" s="14"/>
     </row>
     <row r="116" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A116" s="26"/>
+      <c r="A116" s="29"/>
       <c r="B116" s="24"/>
       <c r="C116" s="10" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="D116" s="10" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="E116" s="10" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="F116" s="10"/>
       <c r="G116" s="14"/>
     </row>
     <row r="117" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="26"/>
+      <c r="A117" s="29"/>
       <c r="B117" s="24"/>
       <c r="C117" s="10" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D117" s="10"/>
       <c r="E117" s="10" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="F117" s="10" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="G117" s="14"/>
     </row>
     <row r="118" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A118" s="26"/>
+      <c r="A118" s="29"/>
       <c r="B118" s="24"/>
       <c r="C118" s="10" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="D118" s="10" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="E118" s="10" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="F118" s="10" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="G118" s="14"/>
     </row>
     <row r="119" spans="1:7" ht="96" x14ac:dyDescent="0.2">
-      <c r="A119" s="26"/>
+      <c r="A119" s="29"/>
       <c r="B119" s="24" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="E119" s="10"/>
       <c r="F119" s="10" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="G119" s="14"/>
     </row>
     <row r="120" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A120" s="26"/>
+      <c r="A120" s="29"/>
       <c r="B120" s="24"/>
       <c r="C120" s="24"/>
       <c r="D120" s="10" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="E120" s="10"/>
       <c r="F120" s="10"/>
       <c r="G120" s="14"/>
     </row>
     <row r="121" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A121" s="26"/>
+      <c r="A121" s="29"/>
       <c r="B121" s="24"/>
       <c r="C121" s="10" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="D121" s="10" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="E121" s="10"/>
       <c r="F121" s="10"/>
       <c r="G121" s="14"/>
     </row>
     <row r="122" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="26"/>
+      <c r="A122" s="29"/>
       <c r="B122" s="24"/>
       <c r="C122" s="10" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="D122" s="24" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="E122" s="10"/>
       <c r="F122" s="10"/>
       <c r="G122" s="14"/>
     </row>
     <row r="123" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="26"/>
+      <c r="A123" s="29"/>
       <c r="B123" s="24"/>
       <c r="C123" s="10" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="D123" s="24"/>
       <c r="E123" s="10"/>
@@ -5674,10 +5674,10 @@
       <c r="G123" s="14"/>
     </row>
     <row r="124" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="26"/>
+      <c r="A124" s="29"/>
       <c r="B124" s="24"/>
       <c r="C124" s="10" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="D124" s="10"/>
       <c r="E124" s="10"/>
@@ -5685,77 +5685,77 @@
       <c r="G124" s="14"/>
     </row>
     <row r="125" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A125" s="26"/>
+      <c r="A125" s="29"/>
       <c r="B125" s="24"/>
       <c r="C125" s="10" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="D125" s="10" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="E125" s="10"/>
       <c r="F125" s="10"/>
       <c r="G125" s="14"/>
     </row>
     <row r="126" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A126" s="26"/>
+      <c r="A126" s="29"/>
       <c r="B126" s="24"/>
       <c r="C126" s="10" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="D126" s="10" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="E126" s="10"/>
       <c r="F126" s="10" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="G126" s="14"/>
     </row>
     <row r="127" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="26"/>
+      <c r="A127" s="29"/>
       <c r="B127" s="24"/>
       <c r="C127" s="10" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="D127" s="10" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="E127" s="10"/>
       <c r="F127" s="10"/>
       <c r="G127" s="14"/>
     </row>
     <row r="128" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A128" s="26"/>
+      <c r="A128" s="29"/>
       <c r="B128" s="24"/>
       <c r="C128" s="10" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="E128" s="10"/>
       <c r="F128" s="10"/>
       <c r="G128" s="14"/>
     </row>
     <row r="129" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="26"/>
+      <c r="A129" s="29"/>
       <c r="B129" s="24"/>
       <c r="C129" s="10" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="D129" s="10" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="E129" s="10"/>
       <c r="F129" s="10"/>
       <c r="G129" s="14"/>
     </row>
     <row r="130" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="26"/>
+      <c r="A130" s="29"/>
       <c r="B130" s="24"/>
       <c r="C130" s="10" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="D130" s="10"/>
       <c r="E130" s="10"/>
@@ -5763,154 +5763,154 @@
       <c r="G130" s="14"/>
     </row>
     <row r="131" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="26"/>
+      <c r="A131" s="29"/>
       <c r="B131" s="24"/>
       <c r="C131" s="10" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="D131" s="10" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="E131" s="10"/>
       <c r="F131" s="10"/>
       <c r="G131" s="14"/>
     </row>
     <row r="132" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="26"/>
+      <c r="A132" s="29"/>
       <c r="B132" s="24" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="C132" s="10" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="D132" s="10" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="E132" s="10" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="F132" s="10"/>
       <c r="G132" s="14"/>
     </row>
     <row r="133" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A133" s="26"/>
+      <c r="A133" s="29"/>
       <c r="B133" s="24"/>
       <c r="C133" s="10" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="D133" s="10" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="E133" s="10"/>
       <c r="F133" s="10"/>
       <c r="G133" s="14"/>
     </row>
     <row r="134" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="26"/>
+      <c r="A134" s="29"/>
       <c r="B134" s="24"/>
       <c r="C134" s="10" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="D134" s="10" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="E134" s="10"/>
       <c r="F134" s="10"/>
       <c r="G134" s="14"/>
     </row>
     <row r="135" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A135" s="26"/>
+      <c r="A135" s="29"/>
       <c r="B135" s="24" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="D135" s="10" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="F135" s="10"/>
       <c r="G135" s="14"/>
     </row>
     <row r="136" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="26"/>
+      <c r="A136" s="29"/>
       <c r="B136" s="24"/>
       <c r="C136" s="10" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="D136" s="10" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="E136" s="10"/>
       <c r="F136" s="10"/>
       <c r="G136" s="14"/>
     </row>
     <row r="137" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A137" s="26"/>
+      <c r="A137" s="29"/>
       <c r="B137" s="24" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="D137" s="10" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="E137" s="10"/>
       <c r="F137" s="10"/>
       <c r="G137" s="14"/>
     </row>
     <row r="138" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A138" s="26"/>
+      <c r="A138" s="29"/>
       <c r="B138" s="24"/>
       <c r="C138" s="10" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="D138" s="10" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="E138" s="10" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="F138" s="10"/>
       <c r="G138" s="14"/>
     </row>
     <row r="139" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A139" s="26"/>
+      <c r="A139" s="29"/>
       <c r="B139" s="24"/>
       <c r="C139" s="10" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="D139" s="10" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="E139" s="10"/>
       <c r="F139" s="10"/>
       <c r="G139" s="14"/>
     </row>
     <row r="140" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A140" s="26"/>
+      <c r="A140" s="29"/>
       <c r="B140" s="24"/>
       <c r="C140" s="10" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="D140" s="10" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="E140" s="10"/>
       <c r="F140" s="10"/>
       <c r="G140" s="14"/>
     </row>
     <row r="141" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="26"/>
+      <c r="A141" s="29"/>
       <c r="B141" s="24" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="D141" s="10"/>
       <c r="E141" s="10"/>
@@ -5918,10 +5918,10 @@
       <c r="G141" s="14"/>
     </row>
     <row r="142" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="27"/>
+      <c r="A142" s="30"/>
       <c r="B142" s="24"/>
       <c r="C142" s="10" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="D142" s="10"/>
       <c r="E142" s="10"/>
@@ -5929,14 +5929,14 @@
       <c r="G142" s="14"/>
     </row>
     <row r="143" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="28" t="s">
-        <v>304</v>
+      <c r="A143" s="25" t="s">
+        <v>315</v>
       </c>
       <c r="B143" s="24" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="C143" s="10" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="D143" s="10"/>
       <c r="E143" s="10"/>
@@ -5944,10 +5944,10 @@
       <c r="G143" s="14"/>
     </row>
     <row r="144" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="29"/>
+      <c r="A144" s="26"/>
       <c r="B144" s="24"/>
       <c r="C144" s="10" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="D144" s="10"/>
       <c r="E144" s="10"/>
@@ -5955,23 +5955,23 @@
       <c r="G144" s="14"/>
     </row>
     <row r="145" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="29"/>
+      <c r="A145" s="26"/>
       <c r="B145" s="24"/>
       <c r="C145" s="10" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="D145" s="10"/>
       <c r="E145" s="10" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="F145" s="14"/>
       <c r="G145" s="14"/>
     </row>
     <row r="146" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="29"/>
+      <c r="A146" s="26"/>
       <c r="B146" s="24"/>
       <c r="C146" s="10" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="D146" s="10"/>
       <c r="E146" s="10"/>
@@ -5979,10 +5979,10 @@
       <c r="G146" s="14"/>
     </row>
     <row r="147" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="29"/>
+      <c r="A147" s="26"/>
       <c r="B147" s="24"/>
       <c r="C147" s="10" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
       <c r="D147" s="10"/>
       <c r="E147" s="10"/>
@@ -5990,10 +5990,10 @@
       <c r="G147" s="14"/>
     </row>
     <row r="148" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="29"/>
+      <c r="A148" s="26"/>
       <c r="B148" s="24"/>
       <c r="C148" s="10" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="D148" s="10"/>
       <c r="E148" s="10"/>
@@ -6001,10 +6001,10 @@
       <c r="G148" s="14"/>
     </row>
     <row r="149" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="29"/>
+      <c r="A149" s="26"/>
       <c r="B149" s="24"/>
       <c r="C149" s="10" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="D149" s="10"/>
       <c r="E149" s="10"/>
@@ -6012,25 +6012,25 @@
       <c r="G149" s="14"/>
     </row>
     <row r="150" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="29"/>
+      <c r="A150" s="26"/>
       <c r="B150" s="24"/>
       <c r="C150" s="10" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="D150" s="10" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="E150" s="10" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="F150" s="14"/>
       <c r="G150" s="14"/>
     </row>
     <row r="151" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A151" s="29"/>
+      <c r="A151" s="26"/>
       <c r="B151" s="24"/>
       <c r="C151" s="10" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="D151" s="10"/>
       <c r="E151" s="10"/>
@@ -6038,25 +6038,25 @@
       <c r="G151" s="14"/>
     </row>
     <row r="152" spans="1:7" ht="80" x14ac:dyDescent="0.2">
-      <c r="A152" s="29"/>
+      <c r="A152" s="26"/>
       <c r="B152" s="24"/>
       <c r="C152" s="10" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="D152" s="10" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="E152" s="10" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="F152" s="14"/>
       <c r="G152" s="14"/>
     </row>
     <row r="153" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="29"/>
+      <c r="A153" s="26"/>
       <c r="B153" s="24"/>
       <c r="C153" s="10" t="s">
-        <v>321</v>
+        <v>332</v>
       </c>
       <c r="D153" s="10"/>
       <c r="E153" s="10"/>
@@ -6064,10 +6064,10 @@
       <c r="G153" s="14"/>
     </row>
     <row r="154" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="29"/>
+      <c r="A154" s="26"/>
       <c r="B154" s="24"/>
       <c r="C154" s="10" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="D154" s="10"/>
       <c r="E154" s="10"/>
@@ -6075,10 +6075,10 @@
       <c r="G154" s="14"/>
     </row>
     <row r="155" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A155" s="29"/>
+      <c r="A155" s="26"/>
       <c r="B155" s="24"/>
       <c r="C155" s="10" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="D155" s="10"/>
       <c r="E155" s="10"/>
@@ -6086,10 +6086,10 @@
       <c r="G155" s="14"/>
     </row>
     <row r="156" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A156" s="29"/>
+      <c r="A156" s="26"/>
       <c r="B156" s="24"/>
       <c r="C156" s="10" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="D156" s="10"/>
       <c r="E156" s="10"/>
@@ -6097,10 +6097,10 @@
       <c r="G156" s="14"/>
     </row>
     <row r="157" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A157" s="29"/>
+      <c r="A157" s="26"/>
       <c r="B157" s="24"/>
       <c r="C157" s="10" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="D157" s="10"/>
       <c r="E157" s="10"/>
@@ -6108,10 +6108,10 @@
       <c r="G157" s="14"/>
     </row>
     <row r="158" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A158" s="29"/>
+      <c r="A158" s="26"/>
       <c r="B158" s="24"/>
       <c r="C158" s="10" t="s">
-        <v>326</v>
+        <v>337</v>
       </c>
       <c r="D158" s="10"/>
       <c r="E158" s="10"/>
@@ -6119,10 +6119,10 @@
       <c r="G158" s="14"/>
     </row>
     <row r="159" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A159" s="29"/>
+      <c r="A159" s="26"/>
       <c r="B159" s="24"/>
       <c r="C159" s="10" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D159" s="10"/>
       <c r="E159" s="10"/>
@@ -6130,10 +6130,10 @@
       <c r="G159" s="14"/>
     </row>
     <row r="160" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A160" s="29"/>
+      <c r="A160" s="26"/>
       <c r="B160" s="24"/>
       <c r="C160" s="10" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="D160" s="10"/>
       <c r="E160" s="10"/>
@@ -6141,42 +6141,42 @@
       <c r="G160" s="14"/>
     </row>
     <row r="161" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A161" s="29"/>
+      <c r="A161" s="26"/>
       <c r="B161" s="24"/>
       <c r="C161" s="10" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="D161" s="10" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="E161" s="10" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="F161" s="14"/>
       <c r="G161" s="14"/>
     </row>
     <row r="162" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A162" s="29"/>
+      <c r="A162" s="26"/>
       <c r="B162" s="24" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="D162" s="10" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="E162" s="10" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="F162" s="14"/>
       <c r="G162" s="14"/>
     </row>
     <row r="163" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A163" s="29"/>
+      <c r="A163" s="26"/>
       <c r="B163" s="24"/>
       <c r="C163" s="10" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="D163" s="10"/>
       <c r="E163" s="10"/>
@@ -6184,10 +6184,10 @@
       <c r="G163" s="14"/>
     </row>
     <row r="164" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A164" s="29"/>
+      <c r="A164" s="26"/>
       <c r="B164" s="24"/>
       <c r="C164" s="10" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="D164" s="10"/>
       <c r="E164" s="10"/>
@@ -6195,10 +6195,10 @@
       <c r="G164" s="14"/>
     </row>
     <row r="165" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="29"/>
+      <c r="A165" s="26"/>
       <c r="B165" s="24"/>
       <c r="C165" s="10" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="D165" s="10"/>
       <c r="E165" s="10"/>
@@ -6206,10 +6206,10 @@
       <c r="G165" s="14"/>
     </row>
     <row r="166" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A166" s="29"/>
+      <c r="A166" s="26"/>
       <c r="B166" s="24"/>
       <c r="C166" s="10" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="D166" s="10"/>
       <c r="E166" s="10"/>
@@ -6217,10 +6217,10 @@
       <c r="G166" s="14"/>
     </row>
     <row r="167" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A167" s="29"/>
+      <c r="A167" s="26"/>
       <c r="B167" s="24"/>
       <c r="C167" s="10" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="D167" s="10"/>
       <c r="E167" s="10"/>
@@ -6228,38 +6228,38 @@
       <c r="G167" s="14"/>
     </row>
     <row r="168" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A168" s="29"/>
+      <c r="A168" s="26"/>
       <c r="B168" s="24"/>
       <c r="C168" s="10" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="D168" s="10" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="E168" s="10" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="F168" s="14"/>
       <c r="G168" s="14"/>
     </row>
     <row r="169" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A169" s="29"/>
+      <c r="A169" s="26"/>
       <c r="B169" s="24"/>
       <c r="C169" s="10" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="D169" s="10"/>
       <c r="E169" s="10" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
       <c r="F169" s="14"/>
       <c r="G169" s="14"/>
     </row>
     <row r="170" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A170" s="29"/>
+      <c r="A170" s="26"/>
       <c r="B170" s="24"/>
       <c r="C170" s="10" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D170" s="10"/>
       <c r="E170" s="10"/>
@@ -6267,10 +6267,10 @@
       <c r="G170" s="14"/>
     </row>
     <row r="171" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="29"/>
+      <c r="A171" s="26"/>
       <c r="B171" s="24"/>
       <c r="C171" s="10" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
       <c r="D171" s="10"/>
       <c r="E171" s="10"/>
@@ -6278,40 +6278,40 @@
       <c r="G171" s="14"/>
     </row>
     <row r="172" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="29"/>
+      <c r="A172" s="26"/>
       <c r="B172" s="24" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="C172" s="10" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="D172" s="10"/>
       <c r="E172" s="10" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="F172" s="14" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="G172" s="14"/>
     </row>
     <row r="173" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="29"/>
+      <c r="A173" s="26"/>
       <c r="B173" s="24"/>
       <c r="C173" s="10" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="D173" s="10"/>
       <c r="E173" s="10"/>
       <c r="F173" s="14" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="G173" s="14"/>
     </row>
     <row r="174" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="29"/>
+      <c r="A174" s="26"/>
       <c r="B174" s="24"/>
       <c r="C174" s="10" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="D174" s="10"/>
       <c r="E174" s="10"/>
@@ -6319,79 +6319,79 @@
       <c r="G174" s="14"/>
     </row>
     <row r="175" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="29"/>
+      <c r="A175" s="26"/>
       <c r="B175" s="24"/>
       <c r="C175" s="10" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="D175" s="10"/>
       <c r="E175" s="10"/>
       <c r="F175" s="14" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="G175" s="14"/>
     </row>
     <row r="176" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="30"/>
+      <c r="A176" s="27"/>
       <c r="B176" s="24"/>
       <c r="C176" s="10" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="D176" s="10"/>
       <c r="E176" s="10"/>
       <c r="F176" s="14" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
       <c r="G176" s="14"/>
     </row>
     <row r="177" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="28" t="s">
-        <v>359</v>
+      <c r="A177" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="B177" s="24" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
       <c r="C177" s="10" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
       <c r="D177" s="10" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="E177" s="10"/>
       <c r="F177" s="14"/>
       <c r="G177" s="14"/>
     </row>
     <row r="178" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A178" s="29"/>
+      <c r="A178" s="26"/>
       <c r="B178" s="24"/>
       <c r="C178" s="10" t="s">
-        <v>363</v>
+        <v>374</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="E178" s="10"/>
       <c r="F178" s="14"/>
       <c r="G178" s="14"/>
     </row>
     <row r="179" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A179" s="29"/>
+      <c r="A179" s="26"/>
       <c r="B179" s="24"/>
       <c r="C179" s="10" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="D179" s="10" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="E179" s="10"/>
       <c r="F179" s="14"/>
       <c r="G179" s="14"/>
     </row>
     <row r="180" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A180" s="29"/>
+      <c r="A180" s="26"/>
       <c r="B180" s="24"/>
       <c r="C180" s="10" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="D180" s="10"/>
       <c r="E180" s="10"/>
@@ -6399,10 +6399,10 @@
       <c r="G180" s="14"/>
     </row>
     <row r="181" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="29"/>
+      <c r="A181" s="26"/>
       <c r="B181" s="24"/>
       <c r="C181" s="10" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="D181" s="10"/>
       <c r="E181" s="10"/>
@@ -6410,10 +6410,10 @@
       <c r="G181" s="14"/>
     </row>
     <row r="182" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="29"/>
+      <c r="A182" s="26"/>
       <c r="B182" s="24"/>
       <c r="C182" s="10" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="D182" s="10"/>
       <c r="E182" s="10"/>
@@ -6421,79 +6421,79 @@
       <c r="G182" s="14"/>
     </row>
     <row r="183" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A183" s="29"/>
+      <c r="A183" s="26"/>
       <c r="B183" s="24" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="C183" s="10" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="E183" s="10"/>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
     </row>
     <row r="184" spans="1:7" ht="80" x14ac:dyDescent="0.2">
-      <c r="A184" s="29"/>
+      <c r="A184" s="26"/>
       <c r="B184" s="24"/>
       <c r="C184" s="10" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="D184" s="10" t="s">
-        <v>374</v>
+        <v>385</v>
       </c>
       <c r="E184" s="10"/>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
     </row>
     <row r="185" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A185" s="29"/>
+      <c r="A185" s="26"/>
       <c r="B185" s="24" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="D185" s="10" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="E185" s="10"/>
       <c r="F185" s="14"/>
       <c r="G185" s="14"/>
     </row>
     <row r="186" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A186" s="29"/>
+      <c r="A186" s="26"/>
       <c r="B186" s="24"/>
       <c r="C186" s="10" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="E186" s="10"/>
       <c r="F186" s="14"/>
       <c r="G186" s="14"/>
     </row>
     <row r="187" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A187" s="29"/>
+      <c r="A187" s="26"/>
       <c r="B187" s="24"/>
       <c r="C187" s="10" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
       <c r="E187" s="10"/>
       <c r="F187" s="14"/>
       <c r="G187" s="14"/>
     </row>
     <row r="188" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="29"/>
+      <c r="A188" s="26"/>
       <c r="B188" s="24"/>
       <c r="C188" s="10" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
       <c r="D188" s="10"/>
       <c r="E188" s="10"/>
@@ -6501,51 +6501,51 @@
       <c r="G188" s="14"/>
     </row>
     <row r="189" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A189" s="29"/>
+      <c r="A189" s="26"/>
       <c r="B189" s="24"/>
       <c r="C189" s="10" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="E189" s="10"/>
       <c r="F189" s="14"/>
       <c r="G189" s="14"/>
     </row>
     <row r="190" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A190" s="29"/>
+      <c r="A190" s="26"/>
       <c r="B190" s="24" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C190" s="10" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
       <c r="E190" s="10"/>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
     </row>
     <row r="191" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A191" s="29"/>
+      <c r="A191" s="26"/>
       <c r="B191" s="24"/>
       <c r="C191" s="10" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="D191" s="10" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
       <c r="E191" s="10"/>
       <c r="F191" s="14"/>
       <c r="G191" s="14"/>
     </row>
     <row r="192" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="30"/>
+      <c r="A192" s="27"/>
       <c r="B192" s="24"/>
       <c r="C192" s="10" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="D192" s="10"/>
       <c r="E192" s="10"/>
@@ -6561,7 +6561,7 @@
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="11"/>
       <c r="B194" s="9" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="C194" s="3"/>
       <c r="D194" s="3"/>
@@ -6569,7 +6569,7 @@
     <row r="195" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A195" s="11"/>
       <c r="B195" s="3" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="C195" s="3"/>
       <c r="D195" s="3"/>
@@ -6577,7 +6577,7 @@
     <row r="196" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A196" s="11"/>
       <c r="B196" s="3" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3"/>
@@ -6585,7 +6585,7 @@
     <row r="197" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A197" s="11"/>
       <c r="B197" s="3" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="C197" s="3"/>
       <c r="D197" s="3"/>
@@ -6593,7 +6593,7 @@
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="11"/>
       <c r="B198" s="3" t="s">
-        <v>395</v>
+        <v>406</v>
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="3"/>
@@ -6601,7 +6601,7 @@
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="11"/>
       <c r="B199" s="3" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="C199" s="3"/>
       <c r="D199" s="3"/>
@@ -6609,7 +6609,7 @@
     <row r="200" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="11"/>
       <c r="B200" s="3" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="3"/>
@@ -6653,13 +6653,12 @@
     <mergeCell ref="A66:A82"/>
     <mergeCell ref="B74:B77"/>
     <mergeCell ref="B78:B82"/>
+    <mergeCell ref="B66:B71"/>
     <mergeCell ref="A2:A20"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B16:B20"/>
     <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B66:B71"/>
-    <mergeCell ref="B94:B95"/>
     <mergeCell ref="A177:A192"/>
     <mergeCell ref="B190:B192"/>
     <mergeCell ref="A143:A176"/>
@@ -6693,6 +6692,7 @@
     <mergeCell ref="B88:B90"/>
     <mergeCell ref="B99:B100"/>
     <mergeCell ref="B96:B98"/>
+    <mergeCell ref="B94:B95"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G29" r:id="rId1"/>
@@ -6714,8 +6714,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5A7A969F2F2324CAA5774C0842691FC" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4da9ab496a844df773281d1737d6c11">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92161533-46f3-49a7-aee7-978486041e93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e14095e5fd45feb9cac09fdddce77b6" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5A7A969F2F2324CAA5774C0842691FC" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b78db5fadbce5c280fe191811afde21">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92161533-46f3-49a7-aee7-978486041e93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1948542ac816cf2454ac8c8e0a0b264f" ns2:_="">
     <xsd:import namespace="92161533-46f3-49a7-aee7-978486041e93"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -6916,7 +6916,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3FD4032-F7EA-4A11-A633-CC8601BCBA1C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA097A21-7F9D-40C0-85B6-697FA2D87221}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>

</xml_diff>